<commit_message>
added graphs regading RUD/kraj/obyvatel
</commit_message>
<xml_diff>
--- a/graphs/graf_A3b.xlsx
+++ b/graphs/graf_A3b.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="B1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,308 +436,68 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Hlavní město Praha</t>
+          <t>Jihomoravský kraj</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Jihomoravský kraj</t>
+          <t>Jihočeský kraj</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Jihočeský kraj</t>
+          <t>Karlovarský kraj</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Karlovarský kraj</t>
+          <t>Kraj Vysočina</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Kraj Vysočina</t>
+          <t>Královéhradecký kraj</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Královéhradecký kraj</t>
+          <t>Liberecký kraj</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Liberecký kraj</t>
+          <t>Moravskoslezský kraj</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Moravskoslezský kraj</t>
+          <t>Olomoucký kraj</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Olomoucký kraj</t>
+          <t>Pardubický kraj</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Pardubický kraj</t>
+          <t>Plzeňský kraj</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Plzeňský kraj</t>
+          <t>Středočeský kraj</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Středočeský kraj</t>
+          <t>Zlínský kraj</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Zlínský kraj</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
           <t>Ústecký kraj</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Předškolní vzdělávání</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>0.1171158482827348</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.4965495772624773</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.003577105917800286</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.06161353921886347</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.004463703070112901</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.176732062737087</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.07452005837627591</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.04809538850133631</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.04989087440251271</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.08014640019316241</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.0006229776985222458</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.04486304628639135</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Základní vzdělávání</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>1.345416719157132</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.761109960488785</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.3680830773256774</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.5723253730952496</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.8531989434766787</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.526433546664449</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.620415133238885</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.8975080206509065</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.5471908571973718</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.7927114530017295</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.7926546885182089</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.6995286693305425</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.7768283646164235</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Střední vzdělávání </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="n">
-        <v>11.90355247443148</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10.29375412896861</v>
-      </c>
-      <c r="E4" t="n">
-        <v>13.95354523504546</v>
-      </c>
-      <c r="F4" t="n">
-        <v>10.12561199964899</v>
-      </c>
-      <c r="G4" t="n">
-        <v>11.0379432769202</v>
-      </c>
-      <c r="H4" t="n">
-        <v>7.959690116222093</v>
-      </c>
-      <c r="I4" t="n">
-        <v>11.16694862730181</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9.91615803412809</v>
-      </c>
-      <c r="K4" t="n">
-        <v>9.934697388320451</v>
-      </c>
-      <c r="L4" t="n">
-        <v>11.00066665499139</v>
-      </c>
-      <c r="M4" t="n">
-        <v>6.688405122357534</v>
-      </c>
-      <c r="N4" t="n">
-        <v>10.1582798743177</v>
-      </c>
-      <c r="O4" t="n">
-        <v>15.67874145195125</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Dětské domovy</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>0.3970912224169427</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8164576363121256</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.9202372195195059</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.720589477854813</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.4719480543779648</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.7371967815707309</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.8774770333958416</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1.480507093732919</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1.719204407403303</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.8062377810274185</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.2879035516381319</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.583299817561579</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1.594077965199519</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Ostatní</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="n">
-        <v>3.497057218704819</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2.672653266201361</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1.182220488161409</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.8631437057371811</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.879079649004745</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.7246591627491014</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3.062119960297261</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1.161484281352513</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.6757389668973961</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1.813109981382544</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.4453842035000326</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.8144021178371834</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.9506215248197792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>